<commit_message>
edit to supplies quotes
</commit_message>
<xml_diff>
--- a/Other/Purchases/20230622_supplies_quotes.xlsx
+++ b/Other/Purchases/20230622_supplies_quotes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3528" yWindow="0" windowWidth="21864" windowHeight="9780"/>
+    <workbookView xWindow="4704" yWindow="0" windowWidth="21864" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="NOAA_DFO supplies" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
   <si>
     <t>Item</t>
   </si>
@@ -111,19 +111,25 @@
     <t>Pierce™ Rapid Gold BCA Protein Assay Kit</t>
   </si>
   <si>
-    <t>A1254301</t>
-  </si>
-  <si>
     <t>A53225</t>
   </si>
   <si>
-    <t>Lab Armor™ Beads</t>
-  </si>
-  <si>
-    <t>4L</t>
-  </si>
-  <si>
-    <t>Lab Armor™ Beads (thermofisher.com)</t>
+    <t>Product Detail (gsaadvantage.gov)</t>
+  </si>
+  <si>
+    <t>LAB ARMOR STAY TEMP TRAY BEADS 4 LITER</t>
+  </si>
+  <si>
+    <t>12L075</t>
+  </si>
+  <si>
+    <t>GSA Advantage</t>
+  </si>
+  <si>
+    <t>tray with beads 4L</t>
+  </si>
+  <si>
+    <t>#003002</t>
   </si>
 </sst>
 </file>
@@ -525,7 +531,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -572,8 +578,8 @@
       <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="5">
-        <v>3002</v>
+      <c r="C2" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>11</v>
@@ -600,7 +606,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>25</v>
@@ -618,111 +624,111 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="5">
-        <v>1</v>
-      </c>
-      <c r="F4" s="5">
-        <v>578</v>
-      </c>
-      <c r="G4" s="5">
-        <v>578</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>32</v>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="5">
+        <v>2</v>
+      </c>
+      <c r="F5" s="5">
+        <v>680</v>
+      </c>
+      <c r="G5" s="5">
+        <f>F5*E5</f>
+        <v>1360</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E6" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" s="5">
-        <v>680</v>
+        <v>340</v>
       </c>
       <c r="G6" s="5">
         <f>F6*E6</f>
-        <v>1360</v>
+        <v>340</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E7" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" s="5">
-        <v>340</v>
+        <v>635</v>
       </c>
       <c r="G7" s="5">
         <f>F7*E7</f>
-        <v>340</v>
+        <v>1270</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="5">
-        <v>2</v>
-      </c>
-      <c r="F8" s="5">
-        <v>635</v>
-      </c>
-      <c r="G8" s="5">
-        <f>F8*E8</f>
-        <v>1270</v>
-      </c>
-      <c r="H8" s="7" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="5">
+        <v>1</v>
+      </c>
+      <c r="F9" s="5">
+        <v>426.38</v>
+      </c>
+      <c r="G9" s="5">
+        <v>426.38</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -733,17 +739,17 @@
     </row>
     <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G12" s="2">
-        <f>SUM(G2:G8)</f>
-        <v>3883.25</v>
+        <f>SUM(G2,G3,G5,G6,G7,G9)</f>
+        <v>3731.63</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" display="https://www.thermofisher.com/order/catalog/product/003002"/>
-    <hyperlink ref="H6" r:id="rId2" display="https://www.abcam.com/products/assay-kits/lipid-peroxidation-mda-assay-kit-colorimetricfluorometric-ab118970.html"/>
-    <hyperlink ref="H8" r:id="rId3" display="https://www.abcam.com/products/assay-kits/atp-assay-kit-colorimetricfluorometric-ab83355.html"/>
+    <hyperlink ref="H5" r:id="rId2" display="https://www.abcam.com/products/assay-kits/lipid-peroxidation-mda-assay-kit-colorimetricfluorometric-ab118970.html"/>
+    <hyperlink ref="H7" r:id="rId3" display="https://www.abcam.com/products/assay-kits/atp-assay-kit-colorimetricfluorometric-ab83355.html"/>
     <hyperlink ref="H3" r:id="rId4" display="https://www.thermofisher.com/order/catalog/product/A53225?SID=srch-srp-A53225"/>
-    <hyperlink ref="H4" r:id="rId5" display="https://www.thermofisher.com/order/catalog/product/A1254302?SID=srch-srp-A1254302"/>
+    <hyperlink ref="H9" r:id="rId5" display="https://www.gsaadvantage.gov/advantage/ws/catalog/product_detail?gsin=11000023477648"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>

</xml_diff>